<commit_message>
finished handling panel and defaults, begin working on coupons
</commit_message>
<xml_diff>
--- a/Spreadsheets/example.xlsx
+++ b/Spreadsheets/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1400" windowWidth="26020" windowHeight="13040"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>UT-NE</t>
   </si>
   <si>
-    <t>blade width (leave blank)</t>
-  </si>
-  <si>
     <t>Defaults</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>width (inches)</t>
+  </si>
+  <si>
+    <t>blade width (leave blank if same)</t>
   </si>
 </sst>
 </file>
@@ -129,8 +129,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -146,15 +148,17 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,7 +455,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="C3:D3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -459,22 +463,21 @@
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>7.0000000000000007E-2</v>
@@ -482,7 +485,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>1.4999999999999999E-2</v>
@@ -490,18 +493,18 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -517,7 +520,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -534,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -581,7 +584,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -592,15 +595,15 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
updated spreadsheet. locked. readme updated. debug output removed from python code
</commit_message>
<xml_diff>
--- a/Spreadsheets/example.xlsx
+++ b/Spreadsheets/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,24 +141,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,10 +457,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -468,7 +473,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -476,7 +481,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1">
@@ -484,26 +489,29 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2"/>
+    </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -519,24 +527,24 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -582,37 +590,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C17" s="1">
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection password="DE8D" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>